<commit_message>
Plots and maps added
</commit_message>
<xml_diff>
--- a/data/merged_data.xlsx
+++ b/data/merged_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,17 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>injured_or_killed_per_1000</t>
+          <t>injured_or_killed_per_10000_per_5_years</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>injured_per_10000</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>killed_per_10000</t>
         </is>
       </c>
     </row>
@@ -481,10 +491,16 @@
         <v>4878</v>
       </c>
       <c r="E2" t="n">
-        <v>4830081</v>
+        <v>4858319</v>
       </c>
       <c r="F2" t="n">
-        <v>1.009920951636215</v>
+        <v>10.04050989653005</v>
+      </c>
+      <c r="G2" t="n">
+        <v>6.170858685895266</v>
+      </c>
+      <c r="H2" t="n">
+        <v>3.86965121063479</v>
       </c>
     </row>
     <row r="3">
@@ -503,10 +519,16 @@
         <v>592</v>
       </c>
       <c r="E3" t="n">
-        <v>737068</v>
+        <v>737857</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8031823386716016</v>
+        <v>8.023234854450118</v>
+      </c>
+      <c r="G3" t="n">
+        <v>4.404647513000486</v>
+      </c>
+      <c r="H3" t="n">
+        <v>3.61858734144963</v>
       </c>
     </row>
     <row r="4">
@@ -525,10 +547,16 @@
         <v>2190</v>
       </c>
       <c r="E4" t="n">
-        <v>6632764</v>
+        <v>6889326</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3301790927583131</v>
+        <v>3.178830556138583</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.590866798871181</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.587963757267402</v>
       </c>
     </row>
     <row r="5">
@@ -547,10 +575,16 @@
         <v>2120</v>
       </c>
       <c r="E5" t="n">
-        <v>2959400</v>
+        <v>2984306</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7163614246130973</v>
+        <v>7.103829164971688</v>
+      </c>
+      <c r="G5" t="n">
+        <v>4.513612210007955</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2.590216954963733</v>
       </c>
     </row>
     <row r="6">
@@ -569,10 +603,16 @@
         <v>13206</v>
       </c>
       <c r="E6" t="n">
-        <v>38260787</v>
+        <v>38960501</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3451575630161502</v>
+        <v>3.389586802284704</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.961987090463749</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.427599711820954</v>
       </c>
     </row>
     <row r="7">
@@ -591,10 +631,16 @@
         <v>1929</v>
       </c>
       <c r="E7" t="n">
-        <v>5269035</v>
+        <v>5485357</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3661011931027218</v>
+        <v>3.516635289189017</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2.065499109720661</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.451136179468355</v>
       </c>
     </row>
     <row r="8">
@@ -613,10 +659,16 @@
         <v>1599</v>
       </c>
       <c r="E8" t="n">
-        <v>3594841</v>
+        <v>3583240</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4448040956470676</v>
+        <v>4.462441812437905</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3.510789118228196</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.9516526942097097</v>
       </c>
     </row>
     <row r="9">
@@ -635,10 +687,16 @@
         <v>1070</v>
       </c>
       <c r="E9" t="n">
-        <v>923576</v>
+        <v>944756</v>
       </c>
       <c r="F9" t="n">
-        <v>1.158540282553899</v>
+        <v>11.32567562418233</v>
+      </c>
+      <c r="G9" t="n">
+        <v>9.028786268623856</v>
+      </c>
+      <c r="H9" t="n">
+        <v>2.296889355558472</v>
       </c>
     </row>
     <row r="10">
@@ -657,10 +715,16 @@
         <v>1874</v>
       </c>
       <c r="E10" t="n">
-        <v>650581</v>
+        <v>678429</v>
       </c>
       <c r="F10" t="n">
-        <v>2.880502197266751</v>
+        <v>27.62263995200677</v>
+      </c>
+      <c r="G10" t="n">
+        <v>20.85700935543734</v>
+      </c>
+      <c r="H10" t="n">
+        <v>6.765630596569427</v>
       </c>
     </row>
     <row r="11">
@@ -679,10 +743,16 @@
         <v>10981</v>
       </c>
       <c r="E11" t="n">
-        <v>19545621</v>
+        <v>20403663</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5618138200878857</v>
+        <v>5.381876773793019</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3.466044307828453</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1.915832465964567</v>
       </c>
     </row>
     <row r="12">
@@ -701,10 +771,16 @@
         <v>6512</v>
       </c>
       <c r="E12" t="n">
-        <v>9972479</v>
+        <v>10240259</v>
       </c>
       <c r="F12" t="n">
-        <v>0.6529971133556661</v>
+        <v>6.359214156595063</v>
+      </c>
+      <c r="G12" t="n">
+        <v>3.960837318665475</v>
+      </c>
+      <c r="H12" t="n">
+        <v>2.398376837929587</v>
       </c>
     </row>
     <row r="13">
@@ -723,10 +799,16 @@
         <v>148</v>
       </c>
       <c r="E13" t="n">
-        <v>1408243</v>
+        <v>1419563</v>
       </c>
       <c r="F13" t="n">
-        <v>0.1050954984331539</v>
+        <v>1.042574369718005</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.5987758204461514</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.4437985492718534</v>
       </c>
     </row>
     <row r="14">
@@ -745,10 +827,16 @@
         <v>315</v>
       </c>
       <c r="E14" t="n">
-        <v>1611206</v>
+        <v>1674001</v>
       </c>
       <c r="F14" t="n">
-        <v>0.1955057267661615</v>
+        <v>1.88171930602192</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.8900831003087811</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.9916362057131387</v>
       </c>
     </row>
     <row r="15">
@@ -767,10 +855,16 @@
         <v>16923</v>
       </c>
       <c r="E15" t="n">
-        <v>12895129</v>
+        <v>12826826</v>
       </c>
       <c r="F15" t="n">
-        <v>1.312356006675079</v>
+        <v>13.19344317916217</v>
+      </c>
+      <c r="G15" t="n">
+        <v>10.53573191060672</v>
+      </c>
+      <c r="H15" t="n">
+        <v>2.657711268555448</v>
       </c>
     </row>
     <row r="16">
@@ -789,10 +883,16 @@
         <v>4564</v>
       </c>
       <c r="E16" t="n">
-        <v>6568713</v>
+        <v>6626443</v>
       </c>
       <c r="F16" t="n">
-        <v>0.6948088613401133</v>
+        <v>6.88755641601384</v>
+      </c>
+      <c r="G16" t="n">
+        <v>4.460915154631225</v>
+      </c>
+      <c r="H16" t="n">
+        <v>2.426641261382615</v>
       </c>
     </row>
     <row r="17">
@@ -811,10 +911,16 @@
         <v>1094</v>
       </c>
       <c r="E17" t="n">
-        <v>3092997</v>
+        <v>3124141</v>
       </c>
       <c r="F17" t="n">
-        <v>0.3537022506003077</v>
+        <v>3.501762564493728</v>
+      </c>
+      <c r="G17" t="n">
+        <v>2.627922363299223</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.8738402011945043</v>
       </c>
     </row>
     <row r="18">
@@ -833,10 +939,16 @@
         <v>1473</v>
       </c>
       <c r="E18" t="n">
-        <v>2893212</v>
+        <v>2905603</v>
       </c>
       <c r="F18" t="n">
-        <v>0.5091227327966288</v>
+        <v>5.069515690891013</v>
+      </c>
+      <c r="G18" t="n">
+        <v>3.204154180732881</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1.865361510158132</v>
       </c>
     </row>
     <row r="19">
@@ -855,10 +967,16 @@
         <v>2960</v>
       </c>
       <c r="E19" t="n">
-        <v>4404659</v>
+        <v>4432764</v>
       </c>
       <c r="F19" t="n">
-        <v>0.6720156997397528</v>
+        <v>6.677549267229205</v>
+      </c>
+      <c r="G19" t="n">
+        <v>4.272729159504093</v>
+      </c>
+      <c r="H19" t="n">
+        <v>2.404820107725112</v>
       </c>
     </row>
     <row r="20">
@@ -877,10 +995,16 @@
         <v>6577</v>
       </c>
       <c r="E20" t="n">
-        <v>4624527</v>
+        <v>4656925</v>
       </c>
       <c r="F20" t="n">
-        <v>1.422199502781582</v>
+        <v>14.12305330234006</v>
+      </c>
+      <c r="G20" t="n">
+        <v>9.444000064420193</v>
+      </c>
+      <c r="H20" t="n">
+        <v>4.679053237919872</v>
       </c>
     </row>
     <row r="21">
@@ -899,10 +1023,16 @@
         <v>244</v>
       </c>
       <c r="E21" t="n">
-        <v>1328009</v>
+        <v>1331961</v>
       </c>
       <c r="F21" t="n">
-        <v>0.1837336945758651</v>
+        <v>1.831885468118061</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.9910200073425572</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.8408654607755032</v>
       </c>
     </row>
     <row r="22">
@@ -921,10 +1051,16 @@
         <v>4858</v>
       </c>
       <c r="E22" t="n">
-        <v>5923188</v>
+        <v>5988171</v>
       </c>
       <c r="F22" t="n">
-        <v>0.8201664373982389</v>
+        <v>8.112660777389289</v>
+      </c>
+      <c r="G22" t="n">
+        <v>5.288760123917637</v>
+      </c>
+      <c r="H22" t="n">
+        <v>2.823900653471653</v>
       </c>
     </row>
     <row r="23">
@@ -943,10 +1079,16 @@
         <v>2173</v>
       </c>
       <c r="E23" t="n">
-        <v>6713315</v>
+        <v>6806028</v>
       </c>
       <c r="F23" t="n">
-        <v>0.3236850944727009</v>
+        <v>3.19275794927673</v>
+      </c>
+      <c r="G23" t="n">
+        <v>2.499255072121361</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.6935028771553688</v>
       </c>
     </row>
     <row r="24">
@@ -965,10 +1107,16 @@
         <v>4578</v>
       </c>
       <c r="E24" t="n">
-        <v>9913065</v>
+        <v>9947064</v>
       </c>
       <c r="F24" t="n">
-        <v>0.4618147868494759</v>
+        <v>4.602363069142815</v>
+      </c>
+      <c r="G24" t="n">
+        <v>3.00591209627283</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1.596450972869984</v>
       </c>
     </row>
     <row r="25">
@@ -987,10 +1135,16 @@
         <v>1377</v>
       </c>
       <c r="E25" t="n">
-        <v>5413479</v>
+        <v>5506968</v>
       </c>
       <c r="F25" t="n">
-        <v>0.2543650765062541</v>
+        <v>2.500468497365519</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1.663347235720273</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.8371212616452466</v>
       </c>
     </row>
     <row r="26">
@@ -1009,10 +1163,16 @@
         <v>3059</v>
       </c>
       <c r="E26" t="n">
-        <v>2988711</v>
+        <v>2987519</v>
       </c>
       <c r="F26" t="n">
-        <v>1.023518165523532</v>
+        <v>10.23926542391864</v>
+      </c>
+      <c r="G26" t="n">
+        <v>6.302888784975091</v>
+      </c>
+      <c r="H26" t="n">
+        <v>3.936376638943551</v>
       </c>
     </row>
     <row r="27">
@@ -1031,10 +1191,16 @@
         <v>5721</v>
       </c>
       <c r="E27" t="n">
-        <v>6040715</v>
+        <v>6080679</v>
       </c>
       <c r="F27" t="n">
-        <v>0.9470733183075183</v>
+        <v>9.40848875594321</v>
+      </c>
+      <c r="G27" t="n">
+        <v>5.895723158548577</v>
+      </c>
+      <c r="H27" t="n">
+        <v>3.512765597394633</v>
       </c>
     </row>
     <row r="28">
@@ -1053,10 +1219,16 @@
         <v>290</v>
       </c>
       <c r="E28" t="n">
-        <v>1013569</v>
+        <v>1036653</v>
       </c>
       <c r="F28" t="n">
-        <v>0.2861176693446623</v>
+        <v>2.797464532490621</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1.311914401443877</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1.485550131046744</v>
       </c>
     </row>
     <row r="29">
@@ -1075,10 +1247,16 @@
         <v>899</v>
       </c>
       <c r="E29" t="n">
-        <v>1865279</v>
+        <v>1897175</v>
       </c>
       <c r="F29" t="n">
-        <v>0.4819654325170659</v>
+        <v>4.738624533846377</v>
+      </c>
+      <c r="G29" t="n">
+        <v>3.552650651626761</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1.185973882219616</v>
       </c>
     </row>
     <row r="30">
@@ -1097,10 +1275,16 @@
         <v>1750</v>
       </c>
       <c r="E30" t="n">
-        <v>2775970</v>
+        <v>2895891</v>
       </c>
       <c r="F30" t="n">
-        <v>0.6304102710043696</v>
+        <v>6.043045128425068</v>
+      </c>
+      <c r="G30" t="n">
+        <v>3.283963381218423</v>
+      </c>
+      <c r="H30" t="n">
+        <v>2.759081747206645</v>
       </c>
     </row>
     <row r="31">
@@ -1119,10 +1303,16 @@
         <v>232</v>
       </c>
       <c r="E31" t="n">
-        <v>1326622</v>
+        <v>1340145</v>
       </c>
       <c r="F31" t="n">
-        <v>0.1748802597876411</v>
+        <v>1.731155957004652</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1.074510594002888</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.6566453630017647</v>
       </c>
     </row>
     <row r="32">
@@ -1141,10 +1331,16 @@
         <v>3708</v>
       </c>
       <c r="E32" t="n">
-        <v>8856972</v>
+        <v>8871970</v>
       </c>
       <c r="F32" t="n">
-        <v>0.4186532372463185</v>
+        <v>4.179455070294422</v>
+      </c>
+      <c r="G32" t="n">
+        <v>2.862949266059286</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1.316505804235136</v>
       </c>
     </row>
     <row r="33">
@@ -1163,10 +1359,16 @@
         <v>1038</v>
       </c>
       <c r="E33" t="n">
-        <v>2092273</v>
+        <v>2091214</v>
       </c>
       <c r="F33" t="n">
-        <v>0.4961111671373669</v>
+        <v>4.963624000221881</v>
+      </c>
+      <c r="G33" t="n">
+        <v>2.596577872948441</v>
+      </c>
+      <c r="H33" t="n">
+        <v>2.36704612727344</v>
       </c>
     </row>
     <row r="34">
@@ -1185,10 +1387,16 @@
         <v>6764</v>
       </c>
       <c r="E34" t="n">
-        <v>19624447</v>
+        <v>19613918</v>
       </c>
       <c r="F34" t="n">
-        <v>0.3446721326720697</v>
+        <v>3.448571570453185</v>
+      </c>
+      <c r="G34" t="n">
+        <v>2.579290889255273</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.8692806811979127</v>
       </c>
     </row>
     <row r="35">
@@ -1207,10 +1415,16 @@
         <v>6854</v>
       </c>
       <c r="E35" t="n">
-        <v>9843336</v>
+        <v>10102084</v>
       </c>
       <c r="F35" t="n">
-        <v>0.6963086498317237</v>
+        <v>6.784738673723164</v>
+      </c>
+      <c r="G35" t="n">
+        <v>4.582222836396926</v>
+      </c>
+      <c r="H35" t="n">
+        <v>2.202515837326239</v>
       </c>
     </row>
     <row r="36">
@@ -1229,10 +1443,16 @@
         <v>199</v>
       </c>
       <c r="E36" t="n">
-        <v>722036</v>
+        <v>746826</v>
       </c>
       <c r="F36" t="n">
-        <v>0.2756095263948058</v>
+        <v>2.664609962695461</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1.7406999756302</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.9239099870652602</v>
       </c>
     </row>
     <row r="37">
@@ -1251,10 +1471,16 @@
         <v>8211</v>
       </c>
       <c r="E37" t="n">
-        <v>11576684</v>
+        <v>11627878</v>
       </c>
       <c r="F37" t="n">
-        <v>0.7092704612132456</v>
+        <v>7.061477597202172</v>
+      </c>
+      <c r="G37" t="n">
+        <v>4.904592222243817</v>
+      </c>
+      <c r="H37" t="n">
+        <v>2.156885374958355</v>
       </c>
     </row>
     <row r="38">
@@ -1273,10 +1499,16 @@
         <v>2491</v>
       </c>
       <c r="E38" t="n">
-        <v>3853214</v>
+        <v>3906463</v>
       </c>
       <c r="F38" t="n">
-        <v>0.6464733077373849</v>
+        <v>6.376612296084718</v>
+      </c>
+      <c r="G38" t="n">
+        <v>3.967783644693422</v>
+      </c>
+      <c r="H38" t="n">
+        <v>2.408828651391297</v>
       </c>
     </row>
     <row r="39">
@@ -1295,10 +1527,16 @@
         <v>1140</v>
       </c>
       <c r="E39" t="n">
-        <v>3922468</v>
+        <v>4052831</v>
       </c>
       <c r="F39" t="n">
-        <v>0.2906333461483943</v>
+        <v>2.812848598917645</v>
+      </c>
+      <c r="G39" t="n">
+        <v>1.712383269867409</v>
+      </c>
+      <c r="H39" t="n">
+        <v>1.100465329050237</v>
       </c>
     </row>
     <row r="40">
@@ -1317,10 +1555,16 @@
         <v>7451</v>
       </c>
       <c r="E40" t="n">
-        <v>12776309</v>
+        <v>12786714</v>
       </c>
       <c r="F40" t="n">
-        <v>0.5831887754123667</v>
+        <v>5.827142141444628</v>
+      </c>
+      <c r="G40" t="n">
+        <v>3.954104236631866</v>
+      </c>
+      <c r="H40" t="n">
+        <v>1.873037904812761</v>
       </c>
     </row>
     <row r="41">
@@ -1339,10 +1583,16 @@
         <v>409</v>
       </c>
       <c r="E41" t="n">
-        <v>1055081</v>
+        <v>1056302</v>
       </c>
       <c r="F41" t="n">
-        <v>0.3876479625734897</v>
+        <v>3.871998727636604</v>
+      </c>
+      <c r="G41" t="n">
+        <v>3.275578385726809</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.5964203419097948</v>
       </c>
     </row>
     <row r="42">
@@ -1361,10 +1611,16 @@
         <v>4694</v>
       </c>
       <c r="E42" t="n">
-        <v>4764080</v>
+        <v>4923837</v>
       </c>
       <c r="F42" t="n">
-        <v>0.9852899195647428</v>
+        <v>9.533215660875857</v>
+      </c>
+      <c r="G42" t="n">
+        <v>6.263407988526021</v>
+      </c>
+      <c r="H42" t="n">
+        <v>3.269807672349836</v>
       </c>
     </row>
     <row r="43">
@@ -1383,10 +1639,16 @@
         <v>204</v>
       </c>
       <c r="E43" t="n">
-        <v>842316</v>
+        <v>859999</v>
       </c>
       <c r="F43" t="n">
-        <v>0.2421893921046258</v>
+        <v>2.372095781506723</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1.325582936724345</v>
+      </c>
+      <c r="H43" t="n">
+        <v>1.046512844782378</v>
       </c>
     </row>
     <row r="44">
@@ -1405,10 +1667,16 @@
         <v>6302</v>
       </c>
       <c r="E44" t="n">
-        <v>6494340</v>
+        <v>6625528</v>
       </c>
       <c r="F44" t="n">
-        <v>0.9703834415814386</v>
+        <v>9.511694766062417</v>
+      </c>
+      <c r="G44" t="n">
+        <v>6.758706626852984</v>
+      </c>
+      <c r="H44" t="n">
+        <v>2.752988139209434</v>
       </c>
     </row>
     <row r="45">
@@ -1427,10 +1695,16 @@
         <v>11152</v>
       </c>
       <c r="E45" t="n">
-        <v>26480266</v>
+        <v>27625500</v>
       </c>
       <c r="F45" t="n">
-        <v>0.4211438057306524</v>
+        <v>4.036850011764493</v>
+      </c>
+      <c r="G45" t="n">
+        <v>2.210276737072632</v>
+      </c>
+      <c r="H45" t="n">
+        <v>1.826573274691861</v>
       </c>
     </row>
     <row r="46">
@@ -1449,10 +1723,16 @@
         <v>684</v>
       </c>
       <c r="E46" t="n">
-        <v>2897640</v>
+        <v>3018802</v>
       </c>
       <c r="F46" t="n">
-        <v>0.2360541682196546</v>
+        <v>2.265799479396132</v>
+      </c>
+      <c r="G46" t="n">
+        <v>1.331654079995972</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.9341453994001594</v>
       </c>
     </row>
     <row r="47">
@@ -1471,10 +1751,16 @@
         <v>130</v>
       </c>
       <c r="E47" t="n">
-        <v>626210</v>
+        <v>624833</v>
       </c>
       <c r="F47" t="n">
-        <v>0.2075980900975711</v>
+        <v>2.080555924543038</v>
+      </c>
+      <c r="G47" t="n">
+        <v>1.168312173012629</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.9122437515304089</v>
       </c>
     </row>
     <row r="48">
@@ -1493,10 +1779,16 @@
         <v>5025</v>
       </c>
       <c r="E48" t="n">
-        <v>8252427</v>
+        <v>8383367</v>
       </c>
       <c r="F48" t="n">
-        <v>0.6089117783168515</v>
+        <v>5.99401171390922</v>
+      </c>
+      <c r="G48" t="n">
+        <v>4.253660850109508</v>
+      </c>
+      <c r="H48" t="n">
+        <v>1.740350863799712</v>
       </c>
     </row>
     <row r="49">
@@ -1515,10 +1807,16 @@
         <v>2140</v>
       </c>
       <c r="E49" t="n">
-        <v>6963985</v>
+        <v>7237383</v>
       </c>
       <c r="F49" t="n">
-        <v>0.3072953201363874</v>
+        <v>2.956869907257913</v>
+      </c>
+      <c r="G49" t="n">
+        <v>1.778267089084549</v>
+      </c>
+      <c r="H49" t="n">
+        <v>1.178602818173365</v>
       </c>
     </row>
     <row r="50">
@@ -1537,10 +1835,16 @@
         <v>984</v>
       </c>
       <c r="E50" t="n">
-        <v>1853914</v>
+        <v>1832961</v>
       </c>
       <c r="F50" t="n">
-        <v>0.5307689569203318</v>
+        <v>5.368362992993304</v>
+      </c>
+      <c r="G50" t="n">
+        <v>3.540719087858389</v>
+      </c>
+      <c r="H50" t="n">
+        <v>1.827643905134916</v>
       </c>
     </row>
     <row r="51">
@@ -1559,10 +1863,16 @@
         <v>2979</v>
       </c>
       <c r="E51" t="n">
-        <v>5736754</v>
+        <v>5769906</v>
       </c>
       <c r="F51" t="n">
-        <v>0.519283204404442</v>
+        <v>5.162995722980583</v>
+      </c>
+      <c r="G51" t="n">
+        <v>3.669037242547799</v>
+      </c>
+      <c r="H51" t="n">
+        <v>1.493958480432783</v>
       </c>
     </row>
     <row r="52">
@@ -1581,10 +1891,16 @@
         <v>125</v>
       </c>
       <c r="E52" t="n">
-        <v>582122</v>
+        <v>581835</v>
       </c>
       <c r="F52" t="n">
-        <v>0.2147316198322688</v>
+        <v>2.148375398523636</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.8937241657858327</v>
+      </c>
+      <c r="H52" t="n">
+        <v>1.254651232737804</v>
       </c>
     </row>
   </sheetData>

</xml_diff>